<commit_message>
R1: Update the sheet 2 of the data dictionary
</commit_message>
<xml_diff>
--- a/Thesis/DataDictionary/FinalDataDictionary.xlsx
+++ b/Thesis/DataDictionary/FinalDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara ghasem pour\GitLab\Path2\Thesis\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE6FAB5-1AB6-4CC4-BD63-DC4962B317C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B6D5FD-F2E0-4419-BDC8-1845A1796D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19695,7 +19695,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A25" sqref="A2:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19728,7 +19728,7 @@
         <v>482</v>
       </c>
       <c r="B2" s="7">
-        <v>3.6802325581395299</v>
+        <v>3.6842105263157898</v>
       </c>
       <c r="C2" s="7">
         <v>4</v>
@@ -19737,7 +19737,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7">
-        <v>1.1171517425022801</v>
+        <v>1.1192102478745301</v>
       </c>
       <c r="F2" s="7">
         <v>173</v>
@@ -19748,7 +19748,7 @@
         <v>506</v>
       </c>
       <c r="B3" s="7">
-        <v>3.4941860465116301</v>
+        <v>3.4970760233918101</v>
       </c>
       <c r="C3" s="7">
         <v>4</v>
@@ -19757,7 +19757,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="7">
-        <v>1.0058140517534799</v>
+        <v>1.0080515218266499</v>
       </c>
       <c r="F3" s="7">
         <v>173</v>
@@ -19768,7 +19768,7 @@
         <v>508</v>
       </c>
       <c r="B4" s="7">
-        <v>2.67441860465116</v>
+        <v>2.6842105263157898</v>
       </c>
       <c r="C4" s="7">
         <v>3</v>
@@ -19777,7 +19777,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="7">
-        <v>1.2229946992001699</v>
+        <v>1.2198055978697699</v>
       </c>
       <c r="F4" s="7">
         <v>173</v>
@@ -19788,7 +19788,7 @@
         <v>512</v>
       </c>
       <c r="B5" s="7">
-        <v>3.93604651162791</v>
+        <v>3.9356725146198799</v>
       </c>
       <c r="C5" s="7">
         <v>4</v>
@@ -19797,7 +19797,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>0.780974468616635</v>
+        <v>0.78325263620524299</v>
       </c>
       <c r="F5" s="7">
         <v>173</v>
@@ -19808,7 +19808,7 @@
         <v>520</v>
       </c>
       <c r="B6" s="7">
-        <v>3.8888888888888902</v>
+        <v>3.9</v>
       </c>
       <c r="C6" s="7">
         <v>4</v>
@@ -19817,7 +19817,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="7">
-        <v>1.0484972127901699</v>
+        <v>1.0414486951431601</v>
       </c>
       <c r="F6" s="7">
         <v>173</v>
@@ -19828,7 +19828,7 @@
         <v>524</v>
       </c>
       <c r="B7" s="7">
-        <v>3.63953488372093</v>
+        <v>3.6315789473684199</v>
       </c>
       <c r="C7" s="7">
         <v>4</v>
@@ -19837,7 +19837,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="7">
-        <v>0.89066360302123604</v>
+        <v>0.88712845970849596</v>
       </c>
       <c r="F7" s="7">
         <v>173</v>
@@ -19848,7 +19848,7 @@
         <v>522</v>
       </c>
       <c r="B8" s="2">
-        <v>2.28488372093023</v>
+        <v>2.2865497076023402</v>
       </c>
       <c r="C8" s="2">
         <v>2</v>
@@ -19857,7 +19857,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <v>1.2910866217115999</v>
+        <v>1.2946929327688801</v>
       </c>
       <c r="F8" s="2">
         <v>173</v>
@@ -19868,7 +19868,7 @@
         <v>514</v>
       </c>
       <c r="B9" s="2">
-        <v>2.3372093023255802</v>
+        <v>2.3333333333333299</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -19877,7 +19877,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <v>1.3077409217843801</v>
+        <v>1.31059034744787</v>
       </c>
       <c r="F9" s="2">
         <v>173</v>
@@ -19888,7 +19888,7 @@
         <v>516</v>
       </c>
       <c r="B10" s="2">
-        <v>3.0406976744185998</v>
+        <v>3.0526315789473699</v>
       </c>
       <c r="C10" s="2">
         <v>3</v>
@@ -19897,7 +19897,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="2">
-        <v>1.04494079487303</v>
+        <v>1.0361873433536599</v>
       </c>
       <c r="F10" s="2">
         <v>173</v>
@@ -19908,7 +19908,7 @@
         <v>502</v>
       </c>
       <c r="B11" s="2">
-        <v>2.3720930232558102</v>
+        <v>2.3742690058479501</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -19917,7 +19917,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="2">
-        <v>1.28914960526169</v>
+        <v>1.2926188274555399</v>
       </c>
       <c r="F11" s="2">
         <v>173</v>
@@ -19928,7 +19928,7 @@
         <v>498</v>
       </c>
       <c r="B12" s="2">
-        <v>2.57558139534884</v>
+        <v>2.57309941520468</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -19937,7 +19937,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="2">
-        <v>1.19945758174772</v>
+        <v>1.2025371641803599</v>
       </c>
       <c r="F12" s="2">
         <v>173</v>
@@ -19948,7 +19948,7 @@
         <v>476</v>
       </c>
       <c r="B13" s="2">
-        <v>2.8779069767441898</v>
+        <v>2.8654970760233902</v>
       </c>
       <c r="C13" s="2">
         <v>3</v>
@@ -19957,7 +19957,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="2">
-        <v>1.26684220046804</v>
+        <v>1.26003368943882</v>
       </c>
       <c r="F13" s="2">
         <v>173</v>
@@ -19968,7 +19968,7 @@
         <v>464</v>
       </c>
       <c r="B14" s="1">
-        <v>3.11046511627907</v>
+        <v>3.1111111111111098</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
@@ -19977,7 +19977,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="1">
-        <v>0.98200523691359098</v>
+        <v>0.98485259837341899</v>
       </c>
       <c r="F14" s="1">
         <v>173</v>
@@ -19988,7 +19988,7 @@
         <v>448</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0526315789473699</v>
+        <v>3.0529411764705898</v>
       </c>
       <c r="C15" s="1">
         <v>3</v>
@@ -19997,7 +19997,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>1.0361873433536599</v>
+        <v>1.0392405323568199</v>
       </c>
       <c r="F15" s="1">
         <v>173</v>
@@ -20008,7 +20008,7 @@
         <v>432</v>
       </c>
       <c r="B16" s="1">
-        <v>3.6162790697674398</v>
+        <v>3.6257309941520499</v>
       </c>
       <c r="C16" s="1">
         <v>4</v>
@@ -20017,7 +20017,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="1">
-        <v>1.0504090503830501</v>
+        <v>1.0461323266476601</v>
       </c>
       <c r="F16" s="1">
         <v>173</v>
@@ -20028,7 +20028,7 @@
         <v>420</v>
       </c>
       <c r="B17" s="1">
-        <v>3.2209302325581399</v>
+        <v>3.2222222222222201</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -20037,7 +20037,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>1.0362004682052199</v>
+        <v>1.0391046925558101</v>
       </c>
       <c r="F17" s="1">
         <v>173</v>
@@ -20048,7 +20048,7 @@
         <v>414</v>
       </c>
       <c r="B18" s="1">
-        <v>3.17441860465116</v>
+        <v>3.1754385964912299</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
@@ -20057,7 +20057,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>1.0889327407162901</v>
+        <v>1.0920483777940999</v>
       </c>
       <c r="F18" s="1">
         <v>173</v>
@@ -20068,7 +20068,7 @@
         <v>532</v>
       </c>
       <c r="B19" s="5">
-        <v>4.0930232558139501</v>
+        <v>4.0994152046783601</v>
       </c>
       <c r="C19" s="5">
         <v>4</v>
@@ -20077,7 +20077,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="5">
-        <v>0.73552951808246603</v>
+        <v>0.73288287131135499</v>
       </c>
       <c r="F19" s="5">
         <v>173</v>
@@ -20088,16 +20088,16 @@
         <v>533</v>
       </c>
       <c r="B20" s="7">
-        <v>3.0662438336856899</v>
+        <v>3.0676058833953599</v>
       </c>
       <c r="C20" s="7">
-        <v>2.9166666666666701</v>
+        <v>2.9166669999999999</v>
       </c>
       <c r="D20" s="7">
         <v>1.75</v>
       </c>
       <c r="E20" s="7">
-        <v>0.67182527425199101</v>
+        <v>0.67356011353767098</v>
       </c>
       <c r="F20" s="7">
         <v>173</v>
@@ -20108,16 +20108,16 @@
         <v>534</v>
       </c>
       <c r="B21" s="2">
-        <v>3.0662438336856899</v>
+        <v>3.0676058833953599</v>
       </c>
       <c r="C21" s="2">
-        <v>2.9166666666666701</v>
+        <v>2.9166669999999999</v>
       </c>
       <c r="D21" s="2">
         <v>1.75</v>
       </c>
       <c r="E21" s="2">
-        <v>0.67182527425199101</v>
+        <v>0.67356011353767098</v>
       </c>
       <c r="F21" s="2">
         <v>173</v>
@@ -20128,7 +20128,7 @@
         <v>535</v>
       </c>
       <c r="B22" s="1">
-        <v>3.2351744186046498</v>
+        <v>3.2377192982456098</v>
       </c>
       <c r="C22" s="1">
         <v>3.2</v>
@@ -20137,7 +20137,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="1">
-        <v>0.54434731972148498</v>
+        <v>0.54491883111867201</v>
       </c>
       <c r="F22" s="1">
         <v>173</v>
@@ -20148,7 +20148,7 @@
         <v>610</v>
       </c>
       <c r="B23" s="5">
-        <v>4.3779069767441898</v>
+        <v>4.39766081871345</v>
       </c>
       <c r="C23" s="5">
         <v>4</v>
@@ -20157,7 +20157,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="5">
-        <v>1.4915670289405001</v>
+        <v>1.47320990942245</v>
       </c>
       <c r="F23" s="5">
         <v>173</v>
@@ -20168,7 +20168,7 @@
         <v>611</v>
       </c>
       <c r="B24" s="5">
-        <v>3.88304093567251</v>
+        <v>3.8941176470588199</v>
       </c>
       <c r="C24" s="5">
         <v>4</v>
@@ -20177,7 +20177,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="5">
-        <v>1.03940259627247</v>
+        <v>1.0323011510943101</v>
       </c>
       <c r="F24" s="5">
         <v>173</v>
@@ -20188,7 +20188,7 @@
         <v>614</v>
       </c>
       <c r="B25" s="5">
-        <v>4.245614035</v>
+        <v>4.2456140350877201</v>
       </c>
       <c r="C25" s="5">
         <v>4</v>
@@ -20197,7 +20197,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="5">
-        <v>1.0999577810000001</v>
+        <v>1.09995778134574</v>
       </c>
       <c r="F25" s="5">
         <v>173</v>

</xml_diff>

<commit_message>
R1:Update data cleaning adding marital status, and update mediation model in the main code
</commit_message>
<xml_diff>
--- a/Thesis/DataDictionary/FinalDataDictionary.xlsx
+++ b/Thesis/DataDictionary/FinalDataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara ghasem pour\GitLab\Path2\Thesis\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B6D5FD-F2E0-4419-BDC8-1845A1796D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8DE4C-E1CB-43D5-9D97-932399E57766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BasicQuestions!$A$1:$A$1017</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3366" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3368" uniqueCount="616">
   <si>
     <t>Question</t>
   </si>
@@ -1897,6 +1910,9 @@
   </si>
   <si>
     <t>control_household</t>
+  </si>
+  <si>
+    <t>relationship_stats</t>
   </si>
 </sst>
 </file>
@@ -2281,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2549,6 +2565,9 @@
       <c r="E9" s="5">
         <v>1</v>
       </c>
+      <c r="F9" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="H9" s="3"/>
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
@@ -3194,104 +3213,104 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="A48" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="5">
         <v>2</v>
       </c>
-      <c r="E48">
-        <v>1</v>
+      <c r="E48" s="5">
+        <v>4</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="A49" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="5">
         <v>3</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D50" s="5">
+        <v>10</v>
+      </c>
+      <c r="E50" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D51" s="5">
+        <v>150</v>
+      </c>
+      <c r="E51" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D52" s="5">
+        <v>6</v>
+      </c>
+      <c r="E52" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B53" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C50" t="s">
-        <v>72</v>
-      </c>
-      <c r="D50">
-        <v>10</v>
-      </c>
-      <c r="E50">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>68</v>
-      </c>
-      <c r="B51" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" t="s">
-        <v>73</v>
-      </c>
-      <c r="D51">
-        <v>150</v>
-      </c>
-      <c r="E51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>68</v>
-      </c>
-      <c r="B52" t="s">
-        <v>69</v>
-      </c>
-      <c r="C52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D52">
-        <v>6</v>
-      </c>
-      <c r="E52">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
-        <v>68</v>
-      </c>
-      <c r="B53" t="s">
-        <v>69</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="C53" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D53">
-        <v>1</v>
-      </c>
-      <c r="E53">
+      <c r="D53" s="5">
+        <v>1</v>
+      </c>
+      <c r="E53" s="5">
         <v>6</v>
       </c>
     </row>
@@ -19692,10 +19711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A2:E25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20200,6 +20219,26 @@
         <v>1.09995778134574</v>
       </c>
       <c r="F25" s="5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>615</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1.3176470588235301</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0.98162725310809995</v>
+      </c>
+      <c r="F26" s="5">
         <v>173</v>
       </c>
     </row>

</xml_diff>

<commit_message>
R1: added child number and child  gender and parent s relationship to child, to main code and data dictionary , updated them again
</commit_message>
<xml_diff>
--- a/Thesis/DataDictionary/FinalDataDictionary.xlsx
+++ b/Thesis/DataDictionary/FinalDataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara ghasem pour\GitLab\Path2\Thesis\DataDictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC8DE4C-E1CB-43D5-9D97-932399E57766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64ABC500-94CA-472E-9173-A6B08D75748C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasicQuestions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3368" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="619">
   <si>
     <t>Question</t>
   </si>
@@ -1913,6 +1913,15 @@
   </si>
   <si>
     <t>relationship_stats</t>
+  </si>
+  <si>
+    <t>control_childnum</t>
+  </si>
+  <si>
+    <t>relation_stats</t>
+  </si>
+  <si>
+    <t>sex_stats</t>
   </si>
 </sst>
 </file>
@@ -1990,7 +1999,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1999,6 +2008,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2297,8 +2307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J1017"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2341,20 +2351,20 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>613</v>
@@ -2373,19 +2383,19 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>130</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>2</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -2405,20 +2415,20 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>41</v>
       </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="E4" s="5">
+        <v>1</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>608</v>
@@ -2492,19 +2502,19 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="8">
         <v>44</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="8">
         <v>1</v>
       </c>
       <c r="F7" s="5" t="s">
@@ -2521,19 +2531,19 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>128</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="8">
         <v>2</v>
       </c>
       <c r="F8" s="5" t="s">
@@ -2550,19 +2560,19 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="8">
         <v>172</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="8">
         <v>1</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -2573,121 +2583,121 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>26</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>80</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>52</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>94</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>78</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="5">
         <v>2</v>
       </c>
     </row>
@@ -19711,10 +19721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19759,7 +19769,7 @@
         <v>1.1192102478745301</v>
       </c>
       <c r="F2" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -19779,7 +19789,7 @@
         <v>1.0080515218266499</v>
       </c>
       <c r="F3" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -19799,7 +19809,7 @@
         <v>1.2198055978697699</v>
       </c>
       <c r="F4" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -19819,7 +19829,7 @@
         <v>0.78325263620524299</v>
       </c>
       <c r="F5" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -19839,7 +19849,7 @@
         <v>1.0414486951431601</v>
       </c>
       <c r="F6" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -19859,7 +19869,7 @@
         <v>0.88712845970849596</v>
       </c>
       <c r="F7" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -19879,7 +19889,7 @@
         <v>1.2946929327688801</v>
       </c>
       <c r="F8" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -19899,7 +19909,7 @@
         <v>1.31059034744787</v>
       </c>
       <c r="F9" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -19919,7 +19929,7 @@
         <v>1.0361873433536599</v>
       </c>
       <c r="F10" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -19939,7 +19949,7 @@
         <v>1.2926188274555399</v>
       </c>
       <c r="F11" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -19959,7 +19969,7 @@
         <v>1.2025371641803599</v>
       </c>
       <c r="F12" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -19979,7 +19989,7 @@
         <v>1.26003368943882</v>
       </c>
       <c r="F13" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -19999,7 +20009,7 @@
         <v>0.98485259837341899</v>
       </c>
       <c r="F14" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -20019,7 +20029,7 @@
         <v>1.0392405323568199</v>
       </c>
       <c r="F15" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -20039,7 +20049,7 @@
         <v>1.0461323266476601</v>
       </c>
       <c r="F16" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -20059,7 +20069,7 @@
         <v>1.0391046925558101</v>
       </c>
       <c r="F17" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -20079,7 +20089,7 @@
         <v>1.0920483777940999</v>
       </c>
       <c r="F18" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -20099,7 +20109,7 @@
         <v>0.73288287131135499</v>
       </c>
       <c r="F19" s="5">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -20119,7 +20129,7 @@
         <v>0.67356011353767098</v>
       </c>
       <c r="F20" s="7">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -20139,7 +20149,7 @@
         <v>0.67356011353767098</v>
       </c>
       <c r="F21" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -20159,7 +20169,7 @@
         <v>0.54491883111867201</v>
       </c>
       <c r="F22" s="1">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -20179,7 +20189,7 @@
         <v>1.47320990942245</v>
       </c>
       <c r="F23" s="5">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -20199,7 +20209,7 @@
         <v>1.0323011510943101</v>
       </c>
       <c r="F24" s="5">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -20219,7 +20229,7 @@
         <v>1.09995778134574</v>
       </c>
       <c r="F25" s="5">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -20239,7 +20249,67 @@
         <v>0.98162725310809995</v>
       </c>
       <c r="F26" s="5">
-        <v>173</v>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="B27" s="5">
+        <v>1.317647059</v>
+      </c>
+      <c r="C27" s="5">
+        <v>1</v>
+      </c>
+      <c r="D27" s="5">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0.98162725299999998</v>
+      </c>
+      <c r="F27" s="5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1.7660818709999999</v>
+      </c>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
+        <v>0.43820002699999999</v>
+      </c>
+      <c r="F28" s="5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1.450292398</v>
+      </c>
+      <c r="C29" s="5">
+        <v>1</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0.498984176</v>
+      </c>
+      <c r="F29" s="5">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>